<commit_message>
fix: import schedule bug
</commit_message>
<xml_diff>
--- a/client/public/templates/agendamentos.xlsx
+++ b/client/public/templates/agendamentos.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Weback\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ScopeSystem\client\public\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A4AFE3AD-240A-4E43-BC8C-B7C7FF9C9F4C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6383162-8F9D-46F6-A0F8-E166FDEED08E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-3045" windowWidth="29040" windowHeight="15720" xr2:uid="{2E23A2F0-7916-498F-87CC-10548E8D6FB9}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{2E23A2F0-7916-498F-87CC-10548E8D6FB9}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="21">
   <si>
     <t>Placa</t>
   </si>
@@ -81,13 +81,31 @@
   </si>
   <si>
     <t>Primeira instalação</t>
+  </si>
+  <si>
+    <t>Prestador</t>
+  </si>
+  <si>
+    <t>Unique Tech</t>
+  </si>
+  <si>
+    <t>10/02/2025</t>
+  </si>
+  <si>
+    <t>Unidas</t>
+  </si>
+  <si>
+    <t>teltonika</t>
+  </si>
+  <si>
+    <t>LM</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -99,6 +117,12 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -126,15 +150,13 @@
   </cellStyleXfs>
   <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -469,24 +491,26 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B39DA93B-0796-4B49-A356-7FE058FFC3E5}">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:I24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+      <selection activeCell="D12" sqref="D12:D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="20" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.26953125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.1796875" customWidth="1"/>
-    <col min="6" max="6" width="14.7265625" customWidth="1"/>
-    <col min="7" max="7" width="10.08984375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="15" customWidth="1"/>
+    <col min="1" max="1" width="8.7265625" style="3"/>
+    <col min="2" max="2" width="20" style="3" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.26953125" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.453125" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.1796875" style="3" customWidth="1"/>
+    <col min="6" max="7" width="14.7265625" style="3" customWidth="1"/>
+    <col min="8" max="8" width="10.08984375" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15" style="3" customWidth="1"/>
+    <col min="10" max="16384" width="8.7265625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="29" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -506,13 +530,16 @@
         <v>5</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" ht="43.5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>
@@ -523,22 +550,664 @@
         <v>10</v>
       </c>
       <c r="D2" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H2" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I2" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="A3" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I3" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="A4" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E4" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I4" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="A5" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G5" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I5" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="A6" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H6" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="A7" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B7" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C7" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H7" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I7" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="A8" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="A9" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C9" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G9" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H9" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I9" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="A10" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C10" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G10" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H10" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="A11" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C11" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D11" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E2" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G2" s="3">
-        <v>46054</v>
-      </c>
-      <c r="H2" s="2" t="s">
+      <c r="E11" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F11" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H11" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I11" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="A12" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F12" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G12" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H12" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="A13" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F13" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G13" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H13" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I13" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="A14" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B14" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H14" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I14" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="A15" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H15" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I15" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="A16" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E16" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H16" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="A17" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B17" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H17" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I17" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="A18" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E18" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H18" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="A19" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E19" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H19" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I19" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="A20" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B20" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H20" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="A21" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B21" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E21" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F21" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G21" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H21" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="A22" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B22" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C22" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F22" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G22" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H22" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="A23" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C23" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E23" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F23" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G23" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H23" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I23" s="2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" ht="29" x14ac:dyDescent="0.35">
+      <c r="A24" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C24" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="F24" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G24" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="H24" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="I24" s="2" t="s">
         <v>14</v>
       </c>
     </row>
   </sheetData>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.511811024" right="0.511811024" top="0.78740157499999996" bottom="0.78740157499999996" header="0.31496062000000002" footer="0.31496062000000002"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
feat: Ui otimization + login page rework
</commit_message>
<xml_diff>
--- a/client/public/templates/agendamentos.xlsx
+++ b/client/public/templates/agendamentos.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29530"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\ScopeSystem\client\public\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4195C75-23B3-4078-8BD5-2E3D47C857A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8359830A-824F-4472-9DCA-BF78F44D29B0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{2E23A2F0-7916-498F-87CC-10548E8D6FB9}"/>
+    <workbookView xWindow="32220" yWindow="3480" windowWidth="14400" windowHeight="7275" xr2:uid="{2E23A2F0-7916-498F-87CC-10548E8D6FB9}"/>
   </bookViews>
   <sheets>
     <sheet name="Planilha1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
   <si>
     <t>Placa</t>
   </si>
@@ -96,6 +96,9 @@
   </si>
   <si>
     <t>331313</t>
+  </si>
+  <si>
+    <t>VehicleGroup</t>
   </si>
 </sst>
 </file>
@@ -488,10 +491,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B39DA93B-0796-4B49-A356-7FE058FFC3E5}">
-  <dimension ref="A1:J2"/>
+  <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G5" sqref="G4:G5"/>
+      <selection activeCell="K2" sqref="K2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -505,10 +508,11 @@
     <col min="8" max="8" width="10.08984375" style="3" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="15" style="3" customWidth="1"/>
     <col min="10" max="10" width="16.6328125" style="3" customWidth="1"/>
-    <col min="11" max="16384" width="8.7265625" style="3"/>
+    <col min="11" max="11" width="15.1796875" style="3" customWidth="1"/>
+    <col min="12" max="16384" width="8.7265625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -539,8 +543,11 @@
       <c r="J1" s="1" t="s">
         <v>18</v>
       </c>
+      <c r="K1" s="1" t="s">
+        <v>20</v>
+      </c>
     </row>
-    <row r="2" spans="1:10" ht="29" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:11" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>8</v>
       </c>

</xml_diff>